<commit_message>
converted this into csv now
</commit_message>
<xml_diff>
--- a/ProcessingSets.xlsx
+++ b/ProcessingSets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="715" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PassengerModes" sheetId="1" r:id="rId1"/>
@@ -628,7 +628,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A12" sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +688,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +843,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A7" sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A5" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1038,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1108,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>